<commit_message>
updates for Ori working remotely
</commit_message>
<xml_diff>
--- a/derivatives/ISTART-ALL-Combined-042122.xlsx
+++ b/derivatives/ISTART-ALL-Combined-042122.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_21e4\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tup54227\Documents\GitHub\istart-sharedreward\derivatives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFBB77EC-E9DC-409D-A32C-588E29B9EA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2264E55D-9B40-425E-A04F-8D11D14CD808}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="1610" windowWidth="14400" windowHeight="9190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="732">
   <si>
     <t>ID</t>
   </si>
@@ -2226,12 +2222,15 @@
   <si>
     <t>Whenever I decided to reject or not, I took anything that seemed a bit fair. Whenever I had to propose an amount to the other person I tied to give the most I could. Whenever it was a triangle, I gave the least.</t>
   </si>
+  <si>
+    <t>sub</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3066,13 +3065,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:RX63"/>
+  <dimension ref="A1:RY63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="RL1" workbookViewId="0">
+      <selection activeCell="RY1" sqref="RY1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:492">
+    <row r="1" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4549,8 +4550,11 @@
       <c r="RX1" t="s">
         <v>491</v>
       </c>
+      <c r="RY1" t="s">
+        <v>731</v>
+      </c>
     </row>
-    <row r="2" spans="1:492">
+    <row r="2" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -6027,8 +6031,11 @@
       <c r="RX2">
         <v>1</v>
       </c>
+      <c r="RY2">
+        <v>1001</v>
+      </c>
     </row>
-    <row r="3" spans="1:492">
+    <row r="3" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -7505,8 +7512,11 @@
       <c r="RX3">
         <v>4</v>
       </c>
+      <c r="RY3">
+        <v>1002</v>
+      </c>
     </row>
-    <row r="4" spans="1:492">
+    <row r="4" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -8983,8 +8993,11 @@
       <c r="RX4">
         <v>1</v>
       </c>
+      <c r="RY4">
+        <v>1003</v>
+      </c>
     </row>
-    <row r="5" spans="1:492">
+    <row r="5" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -10461,8 +10474,11 @@
       <c r="RX5">
         <v>4</v>
       </c>
+      <c r="RY5">
+        <v>1004</v>
+      </c>
     </row>
-    <row r="6" spans="1:492">
+    <row r="6" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1006</v>
       </c>
@@ -11939,8 +11955,11 @@
       <c r="RX6">
         <v>3</v>
       </c>
+      <c r="RY6">
+        <v>1006</v>
+      </c>
     </row>
-    <row r="7" spans="1:492">
+    <row r="7" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1007</v>
       </c>
@@ -13417,8 +13436,11 @@
       <c r="RX7">
         <v>4</v>
       </c>
+      <c r="RY7">
+        <v>1007</v>
+      </c>
     </row>
-    <row r="8" spans="1:492">
+    <row r="8" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1009</v>
       </c>
@@ -14895,8 +14917,11 @@
       <c r="RX8">
         <v>3</v>
       </c>
+      <c r="RY8">
+        <v>1009</v>
+      </c>
     </row>
-    <row r="9" spans="1:492">
+    <row r="9" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1010</v>
       </c>
@@ -16373,8 +16398,11 @@
       <c r="RX9">
         <v>3</v>
       </c>
+      <c r="RY9">
+        <v>1010</v>
+      </c>
     </row>
-    <row r="10" spans="1:492">
+    <row r="10" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1011</v>
       </c>
@@ -17851,8 +17879,11 @@
       <c r="RX10">
         <v>4</v>
       </c>
+      <c r="RY10">
+        <v>1011</v>
+      </c>
     </row>
-    <row r="11" spans="1:492">
+    <row r="11" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1012</v>
       </c>
@@ -19329,8 +19360,11 @@
       <c r="RX11">
         <v>1</v>
       </c>
+      <c r="RY11">
+        <v>1012</v>
+      </c>
     </row>
-    <row r="12" spans="1:492">
+    <row r="12" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1013</v>
       </c>
@@ -20807,8 +20841,11 @@
       <c r="RX12">
         <v>4</v>
       </c>
+      <c r="RY12">
+        <v>1013</v>
+      </c>
     </row>
-    <row r="13" spans="1:492">
+    <row r="13" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1015</v>
       </c>
@@ -22285,8 +22322,11 @@
       <c r="RX13">
         <v>2</v>
       </c>
+      <c r="RY13">
+        <v>1015</v>
+      </c>
     </row>
-    <row r="14" spans="1:492">
+    <row r="14" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1016</v>
       </c>
@@ -23763,8 +23803,11 @@
       <c r="RX14">
         <v>4</v>
       </c>
+      <c r="RY14">
+        <v>1016</v>
+      </c>
     </row>
-    <row r="15" spans="1:492">
+    <row r="15" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1018</v>
       </c>
@@ -25241,8 +25284,11 @@
       <c r="RX15">
         <v>5</v>
       </c>
+      <c r="RY15">
+        <v>1018</v>
+      </c>
     </row>
-    <row r="16" spans="1:492">
+    <row r="16" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1019</v>
       </c>
@@ -26719,8 +26765,11 @@
       <c r="RX16">
         <v>4</v>
       </c>
+      <c r="RY16">
+        <v>1019</v>
+      </c>
     </row>
-    <row r="17" spans="1:492">
+    <row r="17" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1021</v>
       </c>
@@ -28197,8 +28246,11 @@
       <c r="RX17">
         <v>3</v>
       </c>
+      <c r="RY17">
+        <v>1021</v>
+      </c>
     </row>
-    <row r="18" spans="1:492">
+    <row r="18" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1240</v>
       </c>
@@ -29675,8 +29727,11 @@
       <c r="RX18">
         <v>5</v>
       </c>
+      <c r="RY18">
+        <v>1240</v>
+      </c>
     </row>
-    <row r="19" spans="1:492">
+    <row r="19" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1242</v>
       </c>
@@ -31153,8 +31208,11 @@
       <c r="RX19">
         <v>4</v>
       </c>
+      <c r="RY19">
+        <v>1242</v>
+      </c>
     </row>
-    <row r="20" spans="1:492">
+    <row r="20" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1243</v>
       </c>
@@ -32631,8 +32689,11 @@
       <c r="RX20">
         <v>3</v>
       </c>
+      <c r="RY20">
+        <v>1243</v>
+      </c>
     </row>
-    <row r="21" spans="1:492">
+    <row r="21" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1244</v>
       </c>
@@ -34109,8 +34170,11 @@
       <c r="RX21">
         <v>4</v>
       </c>
+      <c r="RY21">
+        <v>1244</v>
+      </c>
     </row>
-    <row r="22" spans="1:492">
+    <row r="22" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1245</v>
       </c>
@@ -35587,8 +35651,11 @@
       <c r="RX22">
         <v>2</v>
       </c>
+      <c r="RY22">
+        <v>1245</v>
+      </c>
     </row>
-    <row r="23" spans="1:492">
+    <row r="23" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1247</v>
       </c>
@@ -37065,8 +37132,11 @@
       <c r="RX23">
         <v>4</v>
       </c>
+      <c r="RY23">
+        <v>1247</v>
+      </c>
     </row>
-    <row r="24" spans="1:492">
+    <row r="24" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1248</v>
       </c>
@@ -38543,8 +38613,11 @@
       <c r="RX24">
         <v>4</v>
       </c>
+      <c r="RY24">
+        <v>1248</v>
+      </c>
     </row>
-    <row r="25" spans="1:492">
+    <row r="25" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1249</v>
       </c>
@@ -40021,8 +40094,11 @@
       <c r="RX25">
         <v>3</v>
       </c>
+      <c r="RY25">
+        <v>1249</v>
+      </c>
     </row>
-    <row r="26" spans="1:492">
+    <row r="26" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1251</v>
       </c>
@@ -41499,8 +41575,11 @@
       <c r="RX26">
         <v>2</v>
       </c>
+      <c r="RY26">
+        <v>1251</v>
+      </c>
     </row>
-    <row r="27" spans="1:492">
+    <row r="27" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1253</v>
       </c>
@@ -42977,8 +43056,11 @@
       <c r="RX27">
         <v>4</v>
       </c>
+      <c r="RY27">
+        <v>1253</v>
+      </c>
     </row>
-    <row r="28" spans="1:492">
+    <row r="28" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1255</v>
       </c>
@@ -44455,8 +44537,11 @@
       <c r="RX28">
         <v>3</v>
       </c>
+      <c r="RY28">
+        <v>1255</v>
+      </c>
     </row>
-    <row r="29" spans="1:492">
+    <row r="29" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1276</v>
       </c>
@@ -45933,8 +46018,11 @@
       <c r="RX29">
         <v>2</v>
       </c>
+      <c r="RY29">
+        <v>1276</v>
+      </c>
     </row>
-    <row r="30" spans="1:492">
+    <row r="30" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1282</v>
       </c>
@@ -47411,8 +47499,11 @@
       <c r="RX30">
         <v>4</v>
       </c>
+      <c r="RY30">
+        <v>1282</v>
+      </c>
     </row>
-    <row r="31" spans="1:492">
+    <row r="31" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1286</v>
       </c>
@@ -48889,8 +48980,11 @@
       <c r="RX31">
         <v>3</v>
       </c>
+      <c r="RY31">
+        <v>1286</v>
+      </c>
     </row>
-    <row r="32" spans="1:492">
+    <row r="32" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1294</v>
       </c>
@@ -50367,8 +50461,11 @@
       <c r="RX32">
         <v>2</v>
       </c>
+      <c r="RY32">
+        <v>1294</v>
+      </c>
     </row>
-    <row r="33" spans="1:492">
+    <row r="33" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1300</v>
       </c>
@@ -51845,8 +51942,11 @@
       <c r="RX33">
         <v>2</v>
       </c>
+      <c r="RY33">
+        <v>1300</v>
+      </c>
     </row>
-    <row r="34" spans="1:492">
+    <row r="34" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1301</v>
       </c>
@@ -53323,8 +53423,11 @@
       <c r="RX34">
         <v>2</v>
       </c>
+      <c r="RY34">
+        <v>1301</v>
+      </c>
     </row>
-    <row r="35" spans="1:492">
+    <row r="35" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1302</v>
       </c>
@@ -54801,8 +54904,11 @@
       <c r="RX35">
         <v>5</v>
       </c>
+      <c r="RY35">
+        <v>1302</v>
+      </c>
     </row>
-    <row r="36" spans="1:492">
+    <row r="36" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1303</v>
       </c>
@@ -56279,8 +56385,11 @@
       <c r="RX36">
         <v>3</v>
       </c>
+      <c r="RY36">
+        <v>1303</v>
+      </c>
     </row>
-    <row r="37" spans="1:492">
+    <row r="37" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>3101</v>
       </c>
@@ -57757,8 +57866,11 @@
       <c r="RX37">
         <v>3</v>
       </c>
+      <c r="RY37">
+        <v>3101</v>
+      </c>
     </row>
-    <row r="38" spans="1:492">
+    <row r="38" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>3116</v>
       </c>
@@ -59235,8 +59347,11 @@
       <c r="RX38">
         <v>3</v>
       </c>
+      <c r="RY38">
+        <v>3116</v>
+      </c>
     </row>
-    <row r="39" spans="1:492">
+    <row r="39" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>3122</v>
       </c>
@@ -60713,8 +60828,11 @@
       <c r="RX39">
         <v>4</v>
       </c>
+      <c r="RY39">
+        <v>3122</v>
+      </c>
     </row>
-    <row r="40" spans="1:492">
+    <row r="40" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>3125</v>
       </c>
@@ -62191,8 +62309,11 @@
       <c r="RX40">
         <v>5</v>
       </c>
+      <c r="RY40">
+        <v>3125</v>
+      </c>
     </row>
-    <row r="41" spans="1:492">
+    <row r="41" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>3140</v>
       </c>
@@ -63669,8 +63790,11 @@
       <c r="RX41">
         <v>3</v>
       </c>
+      <c r="RY41">
+        <v>3140</v>
+      </c>
     </row>
-    <row r="42" spans="1:492">
+    <row r="42" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>3143</v>
       </c>
@@ -65147,8 +65271,11 @@
       <c r="RX42">
         <v>3</v>
       </c>
+      <c r="RY42">
+        <v>3143</v>
+      </c>
     </row>
-    <row r="43" spans="1:492">
+    <row r="43" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>3146</v>
       </c>
@@ -66625,8 +66752,11 @@
       <c r="RX43">
         <v>3</v>
       </c>
+      <c r="RY43">
+        <v>3146</v>
+      </c>
     </row>
-    <row r="44" spans="1:492">
+    <row r="44" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>3152</v>
       </c>
@@ -68103,8 +68233,11 @@
       <c r="RX44">
         <v>4</v>
       </c>
+      <c r="RY44">
+        <v>3152</v>
+      </c>
     </row>
-    <row r="45" spans="1:492">
+    <row r="45" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>3164</v>
       </c>
@@ -69581,8 +69714,11 @@
       <c r="RX45">
         <v>5</v>
       </c>
+      <c r="RY45">
+        <v>3164</v>
+      </c>
     </row>
-    <row r="46" spans="1:492">
+    <row r="46" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>3166</v>
       </c>
@@ -71059,8 +71195,11 @@
       <c r="RX46">
         <v>1</v>
       </c>
+      <c r="RY46">
+        <v>3166</v>
+      </c>
     </row>
-    <row r="47" spans="1:492">
+    <row r="47" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>3167</v>
       </c>
@@ -72537,8 +72676,11 @@
       <c r="RX47">
         <v>2</v>
       </c>
+      <c r="RY47">
+        <v>3167</v>
+      </c>
     </row>
-    <row r="48" spans="1:492">
+    <row r="48" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>3170</v>
       </c>
@@ -74015,8 +74157,11 @@
       <c r="RX48">
         <v>2</v>
       </c>
+      <c r="RY48">
+        <v>3170</v>
+      </c>
     </row>
-    <row r="49" spans="1:492">
+    <row r="49" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>3173</v>
       </c>
@@ -75493,8 +75638,11 @@
       <c r="RX49">
         <v>4</v>
       </c>
+      <c r="RY49">
+        <v>3173</v>
+      </c>
     </row>
-    <row r="50" spans="1:492">
+    <row r="50" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>3175</v>
       </c>
@@ -76971,8 +77119,11 @@
       <c r="RX50">
         <v>2</v>
       </c>
+      <c r="RY50">
+        <v>3175</v>
+      </c>
     </row>
-    <row r="51" spans="1:492">
+    <row r="51" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>3176</v>
       </c>
@@ -78449,8 +78600,11 @@
       <c r="RX51">
         <v>2</v>
       </c>
+      <c r="RY51">
+        <v>3176</v>
+      </c>
     </row>
-    <row r="52" spans="1:492">
+    <row r="52" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>3178</v>
       </c>
@@ -79927,8 +80081,11 @@
       <c r="RX52">
         <v>2</v>
       </c>
+      <c r="RY52">
+        <v>3178</v>
+      </c>
     </row>
-    <row r="53" spans="1:492">
+    <row r="53" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>3186</v>
       </c>
@@ -81405,8 +81562,11 @@
       <c r="RX53">
         <v>5</v>
       </c>
+      <c r="RY53">
+        <v>3186</v>
+      </c>
     </row>
-    <row r="54" spans="1:492">
+    <row r="54" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>3189</v>
       </c>
@@ -82883,8 +83043,11 @@
       <c r="RX54">
         <v>3</v>
       </c>
+      <c r="RY54">
+        <v>3189</v>
+      </c>
     </row>
-    <row r="55" spans="1:492">
+    <row r="55" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>3190</v>
       </c>
@@ -84361,8 +84524,11 @@
       <c r="RX55">
         <v>4</v>
       </c>
+      <c r="RY55">
+        <v>3190</v>
+      </c>
     </row>
-    <row r="56" spans="1:492">
+    <row r="56" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>3199</v>
       </c>
@@ -85839,8 +86005,11 @@
       <c r="RX56">
         <v>3</v>
       </c>
+      <c r="RY56">
+        <v>3199</v>
+      </c>
     </row>
-    <row r="57" spans="1:492">
+    <row r="57" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>3200</v>
       </c>
@@ -87317,8 +87486,11 @@
       <c r="RX57">
         <v>2</v>
       </c>
+      <c r="RY57">
+        <v>3200</v>
+      </c>
     </row>
-    <row r="58" spans="1:492">
+    <row r="58" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>3206</v>
       </c>
@@ -88795,8 +88967,11 @@
       <c r="RX58">
         <v>3</v>
       </c>
+      <c r="RY58">
+        <v>3206</v>
+      </c>
     </row>
-    <row r="59" spans="1:492">
+    <row r="59" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>3210</v>
       </c>
@@ -90273,8 +90448,11 @@
       <c r="RX59">
         <v>4</v>
       </c>
+      <c r="RY59">
+        <v>3210</v>
+      </c>
     </row>
-    <row r="60" spans="1:492">
+    <row r="60" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>3212</v>
       </c>
@@ -91751,8 +91929,11 @@
       <c r="RX60">
         <v>1</v>
       </c>
+      <c r="RY60">
+        <v>3212</v>
+      </c>
     </row>
-    <row r="61" spans="1:492">
+    <row r="61" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>3218</v>
       </c>
@@ -93229,8 +93410,11 @@
       <c r="RX61">
         <v>3</v>
       </c>
+      <c r="RY61">
+        <v>3218</v>
+      </c>
     </row>
-    <row r="62" spans="1:492">
+    <row r="62" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>3220</v>
       </c>
@@ -94707,8 +94891,11 @@
       <c r="RX62">
         <v>3</v>
       </c>
+      <c r="RY62">
+        <v>3220</v>
+      </c>
     </row>
-    <row r="63" spans="1:492">
+    <row r="63" spans="1:493" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>3223</v>
       </c>
@@ -96184,6 +96371,9 @@
       </c>
       <c r="RX63">
         <v>3</v>
+      </c>
+      <c r="RY63">
+        <v>3223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>